<commit_message>
second round of pilot
</commit_message>
<xml_diff>
--- a/musicsyn/questions_after_pilot.xlsx
+++ b/musicsyn/questions_after_pilot.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zofiaholubowska/Documents/PhD/3_experiment/experiment/Results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zofiaholubowska/Documents/PhD/3_experiment/experiment/musicsyn/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2486D2E6-4F8A-7948-B060-2F1B46C35BB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C6F623-E2B9-0747-95B8-4A326827F508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{71475EC1-C435-3843-BA73-A40252A9196E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16240" xr2:uid="{71475EC1-C435-3843-BA73-A40252A9196E}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>Participant</t>
   </si>
@@ -120,6 +120,39 @@
   </si>
   <si>
     <t>P06</t>
+  </si>
+  <si>
+    <t>percpetion bias for different frequencies and loudness</t>
+  </si>
+  <si>
+    <t>yes, yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sound quality was disturbung, </t>
+  </si>
+  <si>
+    <t>regular, easy to follow, predicting the changes</t>
+  </si>
+  <si>
+    <t>difficult, fa</t>
+  </si>
+  <si>
+    <t>sound more enjoyable</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>not natural piano, the sound was not distrubing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">easy to follow, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">addapted, but hard at the beginning, more on the harder side, </t>
+  </si>
+  <si>
+    <t>quick learning phase, where the light is</t>
   </si>
 </sst>
 </file>
@@ -170,7 +203,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -193,11 +226,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -209,6 +253,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -525,10 +572,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30CA642A-A4ED-4D4C-85BA-C43D0BB79962}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -537,7 +584,7 @@
     <col min="2" max="7" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -560,7 +607,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="102" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -573,11 +620,18 @@
       <c r="D2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
+      <c r="E2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="G2" s="4"/>
+      <c r="M2" s="5" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -590,11 +644,15 @@
       <c r="D3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
+      <c r="E3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -605,11 +663,15 @@
         <v>20</v>
       </c>
       <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -622,11 +684,15 @@
       <c r="D5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
+      <c r="E5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -635,11 +701,15 @@
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
+      <c r="E6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -653,8 +723,11 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
+      <c r="J7" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="11" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>21</v>
       </c>

</xml_diff>